<commit_message>
Added way to fit standards as a separate group.
</commit_message>
<xml_diff>
--- a/docs/Examples/CO2_in_Melt_Inclusion_Vapour_Bubbles/Melt_inclusions_all_dimensions.xlsx
+++ b/docs/Examples/CO2_in_Melt_Inclusion_Vapour_Bubbles/Melt_inclusions_all_dimensions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\penny\Box\Berkeley_new\DiadFit_outer\docs\Examples\CO2_in_Melt_Inclusion_Vapour_Bubbles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0FB108C-EC49-4199-BD62-4FD5C243B9E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB132800-391B-4914-80C9-410DE13C978B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{45F1E3FB-C708-426D-8EB9-4F48C45952EA}"/>
+    <workbookView xWindow="28635" yWindow="-165" windowWidth="29130" windowHeight="15810" xr2:uid="{45F1E3FB-C708-426D-8EB9-4F48C45952EA}"/>
   </bookViews>
   <sheets>
     <sheet name="noZ" sheetId="1" r:id="rId1"/>
@@ -491,7 +491,7 @@
   <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -593,8 +593,8 @@
         <v>2.738225629791895</v>
       </c>
       <c r="O2">
-        <f>100000*N2*(F2/H2)</f>
-        <v>3.158276389610029</v>
+        <f>10^4*N2*(F2/(H2/1000))</f>
+        <v>315.82763896100289</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.35">
@@ -642,8 +642,8 @@
         <v>0.18147502903600468</v>
       </c>
       <c r="O3">
-        <f t="shared" ref="O3:O9" si="4">100000*N3*(F3/H3)</f>
-        <v>0.27887057861852432</v>
+        <f t="shared" ref="O3:O9" si="4">10^4*N3*(F3/(H3/1000))</f>
+        <v>27.88705786185243</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.35">
@@ -692,7 +692,7 @@
       </c>
       <c r="O4">
         <f t="shared" si="4"/>
-        <v>0.5092592592592593</v>
+        <v>50.925925925925924</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.35">
@@ -741,7 +741,7 @@
       </c>
       <c r="O5">
         <f t="shared" si="4"/>
-        <v>0.18994627782041443</v>
+        <v>18.994627782041441</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.35">
@@ -790,7 +790,7 @@
       </c>
       <c r="O6">
         <f t="shared" si="4"/>
-        <v>1.8558364712210864</v>
+        <v>185.5836471221086</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.35">
@@ -839,7 +839,7 @@
       </c>
       <c r="O7">
         <f t="shared" si="4"/>
-        <v>3.4379256085789464E-3</v>
+        <v>0.34379256085789467</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.35">
@@ -888,7 +888,7 @@
       </c>
       <c r="O8">
         <f t="shared" si="4"/>
-        <v>0.98546140276172511</v>
+        <v>98.546140276172508</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.35">
@@ -937,7 +937,7 @@
       </c>
       <c r="O9">
         <f t="shared" si="4"/>
-        <v>1.2958739373833713E-3</v>
+        <v>0.12958739373833716</v>
       </c>
     </row>
   </sheetData>

</xml_diff>